<commit_message>
Update python version in Logreg_day1.ipynb
</commit_message>
<xml_diff>
--- a/results/1_table1/table1.xlsx
+++ b/results/1_table1/table1.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -878,47 +878,47 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>hadMeasurmentDayOne, n (%)</t>
+          <t>cad_present, n (%)</t>
         </is>
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>28</v>
+        <v>21366</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>22755 (91.4)</t>
+          <t>3561 (100.0)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>759 (89.6)</t>
+          <t>101 (100.0)</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2710 (91.6)</t>
+          <t>421 (100.0)</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>971 (92.0)</t>
+          <t>140 (100.0)</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>18315 (91.4)</t>
+          <t>2899 (100.0)</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>cad_present, n (%)</t>
+          <t>heart_failure_present, n (%)</t>
         </is>
       </c>
       <c r="B15" s="1" t="inlineStr">
@@ -927,38 +927,38 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>21366</v>
+        <v>21263</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>3561 (100.0)</t>
+          <t>3664 (100.0)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>101 (100.0)</t>
+          <t>117 (100.0)</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>421 (100.0)</t>
+          <t>544 (100.0)</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>140 (100.0)</t>
+          <t>159 (100.0)</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2899 (100.0)</t>
+          <t>2844 (100.0)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>heart_failure_present, n (%)</t>
+          <t>hypertension_present, n (%)</t>
         </is>
       </c>
       <c r="B16" s="1" t="inlineStr">
@@ -967,183 +967,263 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>21263</v>
+        <v>18767</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>3664 (100.0)</t>
+          <t>6160 (100.0)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>117 (100.0)</t>
+          <t>195 (100.0)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>544 (100.0)</t>
+          <t>918 (100.0)</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>159 (100.0)</t>
+          <t>242 (100.0)</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2844 (100.0)</t>
+          <t>4805 (100.0)</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>hypertension_present, n (%)</t>
-        </is>
-      </c>
-      <c r="B17" s="1" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+          <t>totalinsulin_perLOS, median [Q1,Q3]</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr"/>
       <c r="C17" t="n">
-        <v>18767</v>
+        <v>10556</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>6160 (100.0)</t>
+          <t>12.2 [3.0,35.5]</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>195 (100.0)</t>
+          <t>9.8 [2.9,25.7]</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>918 (100.0)</t>
+          <t>9.2 [2.5,28.4]</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>242 (100.0)</t>
+          <t>15.1 [4.1,40.9]</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>4805 (100.0)</t>
+          <t>12.6 [3.1,36.5]</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>totalinsulin_perLOS, median [Q1,Q3]</t>
-        </is>
-      </c>
-      <c r="B18" s="1" t="inlineStr"/>
+          <t>english_Proficent, n (%)</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C18" t="n">
-        <v>10556</v>
+        <v>0</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>12.2 [3.0,35.5]</t>
+          <t>22486 (90.2)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>9.8 [2.9,25.7]</t>
+          <t>320 (37.8)</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>9.2 [2.5,28.4]</t>
+          <t>2654 (89.6)</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>15.1 [4.1,40.9]</t>
+          <t>415 (39.3)</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>12.6 [3.1,36.5]</t>
+          <t>19097 (95.2)</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>english_Proficent, n (%)</t>
-        </is>
-      </c>
-      <c r="B19" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>methylprednisolone_equivalent_normalized_by_icu_los, mean (SD)</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr"/>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>22712</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>22486 (90.2)</t>
+          <t>57.6 (94.5)</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>320 (37.8)</t>
+          <t>52.9 (63.2)</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2654 (89.6)</t>
+          <t>46.9 (58.8)</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>415 (39.3)</t>
+          <t>84.2 (131.9)</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>19097 (95.2)</t>
+          <t>57.9 (97.6)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>methylprednisolone_equivalent_normalized_by_icu_los, mean (SD)</t>
-        </is>
-      </c>
-      <c r="B20" s="1" t="inlineStr"/>
+          <t>hadMeasurmentDayOne_chart, n (%)</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
       <c r="C20" t="n">
-        <v>22712</v>
+        <v>28</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>57.6 (94.5)</t>
+          <t>22755 (91.4)</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>52.9 (63.2)</t>
+          <t>759 (89.6)</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>46.9 (58.8)</t>
+          <t>2710 (91.6)</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>84.2 (131.9)</t>
+          <t>971 (92.0)</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>57.9 (97.6)</t>
+          <t>18315 (91.4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>hadMeasurmentDayOne_lab, n (%)</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>28</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>22755 (91.4)</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>759 (89.6)</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2710 (91.6)</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>971 (92.0)</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>18315 (91.4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>measurment_before, n (%)</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>23326</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>1601 (100.0)</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>68 (100.0)</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>253 (100.0)</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>112 (100.0)</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>1168 (100.0)</t>
         </is>
       </c>
     </row>

</xml_diff>